<commit_message>
Controle dos bancos de dados
</commit_message>
<xml_diff>
--- a/Banco de dados/Pesquisa Rolf.xlsx
+++ b/Banco de dados/Pesquisa Rolf.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27a8628a50772066/R/ICSAP/Banco de dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{88AEFC9C-1FCA-4A2A-A546-7F1F4EB77DEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:40009_{88AEFC9C-1FCA-4A2A-A546-7F1F4EB77DEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5B4C7DC1-2B24-4BCB-BB5F-174D315DC2D1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pesquisa Rolf" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t xml:space="preserve"> Morbidade Hospitalar do SUS - por local de internação - Brasil</t>
   </si>
@@ -52,9 +63,6 @@
     <t>Rolf 2</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Fonte: Ministério da Saúde - Sistema de Informações Hospitalares do SUS (SIH/SUS)</t>
   </si>
   <si>
@@ -68,12 +76,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Dados de janeiro de 2015 até março de 2016 sujeitos a retificação.</t>
+  </si>
+  <si>
+    <t>Extraído csv</t>
+  </si>
+  <si>
+    <t>SIM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,7 +614,15 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -909,11 +931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,24 +943,26 @@
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -960,8 +984,11 @@
       <c r="J4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2008</v>
       </c>
@@ -992,11 +1019,12 @@
       <c r="J5" s="1">
         <v>11107155</v>
       </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" t="str">
+        <f t="shared" ref="K5:K11" si="0">IF(J5=F5,"OK","DEU RUIM")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2009</v>
       </c>
@@ -1024,8 +1052,18 @@
       <c r="I6" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <v>11511559</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2010</v>
       </c>
@@ -1056,11 +1094,15 @@
       <c r="J7" s="1">
         <v>11724834</v>
       </c>
-      <c r="K7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2011</v>
       </c>
@@ -1091,11 +1133,15 @@
       <c r="J8" s="1">
         <v>11643468</v>
       </c>
-      <c r="K8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2012</v>
       </c>
@@ -1123,8 +1169,15 @@
       <c r="I9" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="1">
+        <v>11429889</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>DEU RUIM</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -1152,8 +1205,15 @@
       <c r="I10" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="1">
+        <v>11024228</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>DEU RUIM</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2014</v>
       </c>
@@ -1181,8 +1241,18 @@
       <c r="I11" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="1">
+        <v>11612715</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -1211,7 +1281,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2016</v>
       </c>
@@ -1240,7 +1310,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -1268,8 +1338,18 @@
       <c r="I14" s="2">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="1">
+        <v>11675269</v>
+      </c>
+      <c r="K14" t="str">
+        <f>IF(J14=F14,"OK","DEU RUIM")</f>
+        <v>OK</v>
+      </c>
+      <c r="L14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2018</v>
       </c>
@@ -1297,8 +1377,15 @@
       <c r="I15" s="2">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="1">
+        <v>8966476</v>
+      </c>
+      <c r="K15" t="str">
+        <f>IF(J15=F15,"OK","DEU RUIM")</f>
+        <v>DEU RUIM</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -1345,35 +1432,40 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K5:K15">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="RUIM">
+      <formula>NOT(ISERROR(SEARCH("RUIM",K5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>